<commit_message>
add new lines to the database: SS-x (d250 135 gr), SS-x (d250 150 gr)
</commit_message>
<xml_diff>
--- a/product_list.xlsx
+++ b/product_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="485"/>
   </bookViews>
   <sheets>
     <sheet name="odr" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Метал">base!$M$2:$M$4</definedName>
     <definedName name="Металл">base!$M$2:$M$4</definedName>
-    <definedName name="Самотечка">base!$A$2:$A$189</definedName>
+    <definedName name="Самотечка">base!$A$2:$A$191</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
   <si>
     <t>DXF</t>
   </si>
@@ -1005,6 +1005,33 @@
   </si>
   <si>
     <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-Х (д160 45 гр)\чертежи сварка</t>
+  </si>
+  <si>
+    <t>СС-х (д250 135 гр)</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-х (д250 135 гр)\DXF</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-х (д250 135 гр)\Заявка СС-135 №хх от 00.00.2021.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-х (д250 135 гр)\чертежи сварка</t>
+  </si>
+  <si>
+    <t>СС-х (д250 150 гр)</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-х (д250 150 гр)\DXF</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-х (д250 150 гр)\Заявка СС-150 №хх от 00.00.2021.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\СС-х (д250 150 гр)\чертежи сварка</t>
+  </si>
+  <si>
+    <t>нержавейка</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1408,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1497,6 +1524,9 @@
       <c r="E4" s="10" t="s">
         <v>250</v>
       </c>
+      <c r="M4" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -2291,301 +2321,305 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="B52" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="C52" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="7" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>161</v>
+        <v>329</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>330</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>331</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="7" t="s">
-        <v>164</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B54" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C54" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="7" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>142</v>
+        <v>308</v>
       </c>
       <c r="B56" t="s">
-        <v>141</v>
+        <v>309</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>310</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="7" t="s">
-        <v>144</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>304</v>
+        <v>168</v>
       </c>
       <c r="B57" t="s">
-        <v>305</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
-        <v>306</v>
+        <v>170</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="7" t="s">
-        <v>307</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>286</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>288</v>
+        <v>143</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="7" t="s">
-        <v>289</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>19</v>
+        <v>304</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>305</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>306</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="7" t="s">
-        <v>69</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>172</v>
+        <v>286</v>
       </c>
       <c r="B60" t="s">
-        <v>173</v>
+        <v>287</v>
       </c>
       <c r="C60" t="s">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="7" t="s">
-        <v>175</v>
+        <v>289</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>176</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>35</v>
       </c>
       <c r="C61" t="s">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="7" t="s">
-        <v>179</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="B62" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="7" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>312</v>
+        <v>176</v>
       </c>
       <c r="B63" t="s">
-        <v>313</v>
+        <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>314</v>
+        <v>178</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="7" t="s">
-        <v>315</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>154</v>
+        <v>36</v>
       </c>
       <c r="C64" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="7" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="B65" t="s">
-        <v>262</v>
+        <v>313</v>
       </c>
       <c r="C65" t="s">
-        <v>263</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F65" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="7" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="B66" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="C66" t="s">
-        <v>49</v>
-      </c>
-      <c r="D66" t="s">
-        <v>50</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>68</v>
+        <v>155</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>99</v>
+        <v>261</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>262</v>
       </c>
       <c r="C67" t="s">
-        <v>101</v>
-      </c>
-      <c r="D67" t="s">
-        <v>102</v>
+        <v>263</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>103</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="F67" s="7"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>165</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>167</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="D68" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>180</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>100</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
-      </c>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="D69" t="s">
+        <v>102</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>220</v>
+        <v>165</v>
       </c>
       <c r="B70" t="s">
-        <v>221</v>
+        <v>166</v>
       </c>
       <c r="C70" t="s">
-        <v>222</v>
+        <v>167</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -2593,13 +2627,13 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2607,17 +2641,45 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>104</v>
+        <v>220</v>
       </c>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>221</v>
       </c>
       <c r="C72" t="s">
-        <v>106</v>
+        <v>222</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" t="s">
+        <v>218</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" t="s">
+        <v>106</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:J44">

</xml_diff>

<commit_message>
add some new position in product_list.xlsx/base
</commit_message>
<xml_diff>
--- a/product_list.xlsx
+++ b/product_list.xlsx
@@ -16,9 +16,9 @@
     <sheet name="base" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Метал">base!$M$2:$M$4</definedName>
-    <definedName name="Металл">base!$M$2:$M$4</definedName>
-    <definedName name="Самотечка">base!$A$2:$A$191</definedName>
+    <definedName name="Метал">base!$M$2:$M$5</definedName>
+    <definedName name="Металл">base!$M$2:$M$5</definedName>
+    <definedName name="Самотечка">base!$A$2:$A$194</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="348">
   <si>
     <t>DXF</t>
   </si>
@@ -1032,6 +1032,48 @@
   </si>
   <si>
     <t>нержавейка</t>
+  </si>
+  <si>
+    <t>СП-9 (300х300-ф300 Н170)</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н170)\DXF</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н170)\СП-9 h170 Заявка №хх от 00.00.2021.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н170)\чертежи гибка</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н170)\чертежи сварка</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н50)\DXF</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н50)\СП-9 h50 №хх от 00.00.2021.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\Самотёки, переходы\Патрубок переходной СП-9 (300х300-ф300 Н50)\чертежи сварка</t>
+  </si>
+  <si>
+    <t>СП-9 (300х300-ф300 Н50</t>
+  </si>
+  <si>
+    <t>ЗВР-300 h80</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\ЗАДВИЖКИ\ЗВР-300 h80\DXF</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\ЗАДВИЖКИ\ЗВР-300 h80\Заявка ЗВР-300 №хх от 00.00.2021.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\ЗАДВИЖКИ\ЗВР-300 h80\Заказ снабжение ЗВР-300.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Рабочая\САМОТЕЧНОЕ ОБОРУДОВАНИЕ\ЗАДВИЖКИ\ЗВР-300 h80\чертежи гибка</t>
   </si>
 </sst>
 </file>
@@ -1435,10 +1477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:XFD62"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,1178 +1532,1187 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>252</v>
+        <v>343</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>251</v>
+        <v>344</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>253</v>
+        <v>345</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>255</v>
+        <v>346</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="M3" t="s">
-        <v>5</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="M4" t="s">
-        <v>333</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>285</v>
+        <v>250</v>
+      </c>
+      <c r="M5" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>86</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>295</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>297</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>298</v>
+        <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>299</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="C15" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="D15" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>256</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>258</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>259</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>55</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>274</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>275</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>276</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>277</v>
+        <v>54</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>278</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>275</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>62</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>290</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>291</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>292</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>293</v>
+        <v>81</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>294</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>16</v>
+        <v>290</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>291</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>292</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>293</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>65</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="7" t="s">
-        <v>72</v>
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>133</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="7" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>227</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>228</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>229</v>
+        <v>131</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="6" t="s">
-        <v>230</v>
-      </c>
+      <c r="E30" s="2"/>
       <c r="F30" s="7" t="s">
-        <v>231</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B31" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C31" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="6" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B32" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C32" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="6" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="B33" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="C33" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="6" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>316</v>
+        <v>269</v>
       </c>
       <c r="B34" t="s">
-        <v>317</v>
+        <v>270</v>
       </c>
       <c r="C34" t="s">
-        <v>318</v>
+        <v>271</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="6" t="s">
-        <v>319</v>
+        <v>272</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>320</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>145</v>
+        <v>316</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>317</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>318</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="6" t="s">
-        <v>148</v>
+        <v>319</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>149</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="6" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="6" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B38" t="s">
+        <v>339</v>
+      </c>
+      <c r="C38" t="s">
+        <v>340</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B40" t="s">
+        <v>335</v>
+      </c>
+      <c r="C40" t="s">
+        <v>336</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>223</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>224</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="6" t="s">
+      <c r="D41" s="2"/>
+      <c r="E41" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" t="s">
-        <v>185</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B40" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" t="s">
-        <v>189</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B41" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" t="s">
-        <v>193</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="7" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>321</v>
+        <v>183</v>
       </c>
       <c r="B42" t="s">
-        <v>322</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
-        <v>323</v>
+        <v>185</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="7" t="s">
-        <v>324</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B43" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="C43" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="7" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>200</v>
+      <c r="A44" s="9" t="s">
+        <v>192</v>
       </c>
       <c r="B44" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="7" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>208</v>
+        <v>321</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>322</v>
       </c>
       <c r="C45" t="s">
-        <v>210</v>
+        <v>323</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="7" t="s">
-        <v>211</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>157</v>
+      <c r="A46" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C46" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="7" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="B47" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>202</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="7" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>21</v>
+      <c r="A48" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>210</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="7" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="7" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>242</v>
+        <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>243</v>
+        <v>138</v>
       </c>
       <c r="C50" t="s">
-        <v>244</v>
+        <v>139</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="7" t="s">
-        <v>245</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>212</v>
+      <c r="A51" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>213</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>214</v>
+        <v>40</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="7" t="s">
-        <v>215</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>325</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>326</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>327</v>
+        <v>42</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="7" t="s">
-        <v>328</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="B53" t="s">
-        <v>330</v>
+        <v>243</v>
       </c>
       <c r="C53" t="s">
-        <v>331</v>
+        <v>244</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="7" t="s">
-        <v>332</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>300</v>
+      <c r="A54" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>301</v>
+        <v>213</v>
       </c>
       <c r="C54" t="s">
-        <v>302</v>
+        <v>214</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="7" t="s">
-        <v>303</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>161</v>
+        <v>325</v>
       </c>
       <c r="B55" t="s">
-        <v>162</v>
+        <v>326</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="7" t="s">
-        <v>164</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="B56" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="C56" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="7" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>168</v>
+        <v>300</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>301</v>
       </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>302</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="7" t="s">
-        <v>171</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="C58" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="7" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B59" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C59" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="7" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>286</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s">
-        <v>287</v>
+        <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>288</v>
+        <v>170</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="7" t="s">
-        <v>289</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="7" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>172</v>
+        <v>304</v>
       </c>
       <c r="B62" t="s">
-        <v>173</v>
+        <v>305</v>
       </c>
       <c r="C62" t="s">
-        <v>174</v>
+        <v>306</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="7" t="s">
-        <v>175</v>
+        <v>307</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>176</v>
+        <v>286</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>287</v>
       </c>
       <c r="C63" t="s">
-        <v>178</v>
+        <v>288</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="7" t="s">
-        <v>179</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>312</v>
+        <v>172</v>
       </c>
       <c r="B65" t="s">
-        <v>313</v>
+        <v>173</v>
       </c>
       <c r="C65" t="s">
-        <v>314</v>
+        <v>174</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="7" t="s">
-        <v>315</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="C66" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="7" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>261</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>262</v>
+        <v>36</v>
       </c>
       <c r="C67" t="s">
-        <v>263</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F67" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>47</v>
+        <v>312</v>
       </c>
       <c r="B68" t="s">
-        <v>48</v>
+        <v>313</v>
       </c>
       <c r="C68" t="s">
-        <v>49</v>
-      </c>
-      <c r="D68" t="s">
-        <v>50</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>68</v>
+        <v>314</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="7" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
-      </c>
-      <c r="D69" t="s">
-        <v>102</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>103</v>
+        <v>155</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>165</v>
+        <v>261</v>
       </c>
       <c r="B70" t="s">
-        <v>166</v>
+        <v>262</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+        <v>263</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F70" s="7"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>180</v>
+        <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>48</v>
       </c>
       <c r="C71" t="s">
-        <v>182</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="D71" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>100</v>
       </c>
       <c r="C72" t="s">
-        <v>222</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="D72" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -2669,17 +2720,59 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>104</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>182</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B75" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" t="s">
+        <v>222</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B76" t="s">
+        <v>217</v>
+      </c>
+      <c r="C76" t="s">
+        <v>218</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" t="s">
+        <v>105</v>
+      </c>
+      <c r="C77" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:J44">

</xml_diff>